<commit_message>
updated for JSON 2
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MahiWay\Desktop\Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chanchal\AutomationTool\Spring Tool Suite 4\JsonTool\JsonTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B103B8-4956-4C79-926E-AFA7340DC21B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1260" windowWidth="20520" windowHeight="11100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1530" yWindow="1260" windowWidth="20520" windowHeight="11100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Complete</t>
   </si>
@@ -110,36 +108,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>dist_refid</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>features</t>
-  </si>
-  <si>
-    <t>[{"name":"share","options":["google|microsoft|hmh|other"]}]</t>
-  </si>
-  <si>
-    <t>Garden Grove USD (96011.0)</t>
-  </si>
-  <si>
-    <t>Brea Olinda Unified School District (94908.0)</t>
-  </si>
-  <si>
-    <t>Central USD (58980.0)</t>
-  </si>
-  <si>
-    <t>Rosedale USD (63727.0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,22 +460,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3838EE58-4CF5-46D7-A79C-EFC955DDCCE9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="36" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -521,7 +495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42377</v>
       </c>
@@ -541,7 +515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42377</v>
       </c>
@@ -561,7 +535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42377</v>
       </c>
@@ -581,7 +555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42377</v>
       </c>
@@ -601,7 +575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42377</v>
       </c>
@@ -621,7 +595,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42377</v>
       </c>
@@ -641,7 +615,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42377</v>
       </c>
@@ -661,7 +635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>42377</v>
       </c>
@@ -681,7 +655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42377</v>
       </c>
@@ -705,92 +679,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E35D4A-41CE-42DC-B7E5-914D5CC92AED}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>